<commit_message>
0926 mini board com
</commit_message>
<xml_diff>
--- a/side_project/mini_board/doc/설계서_mini_boards_ver.1.0.0.xlsx
+++ b/side_project/mini_board/doc/설계서_mini_boards_ver.1.0.0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\2308_php\side_project\mini_board\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="21795" windowHeight="13875" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="21795" windowHeight="13875"/>
   </bookViews>
   <sheets>
     <sheet name="delete(게시판삭제기능)" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="159">
   <si>
     <t>파일명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,9 +68,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>boolen</t>
-  </si>
-  <si>
     <t>파라미터</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -211,92 +208,432 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;$array_param</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$array_param["id"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPDATE boards</t>
+  </si>
+  <si>
+    <t>boards</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 테이블</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SET</t>
+  </si>
+  <si>
+    <t>delete_at = now()</t>
+  </si>
+  <si>
+    <t>WHERE</t>
+  </si>
+  <si>
+    <t>id = :id</t>
+  </si>
+  <si>
+    <t>:id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. sql 작성 (UPDATE)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>2. Query 실행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$stmt = $conn-&gt;prepare($sql);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$result = $stmt-&gt;execute($arr_ps);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prepared Statment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. return 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-1. Instance 생성 정상 처리 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-2. Instance 생성 에러 발생 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-1. [2] 까지 작업이 정상 종료 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>retrun false;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return $result;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-2. [2] 까지 작업에서 에러 발생 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mini_board/src/delete.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mini_board/src/lib/lib_db.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판 삭제 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 설정 정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>define("ROOT", $_SERVER["DOCUMENT_ROOT"]."/mini_board/src/"); // 웹서버 root 패스 생성</t>
+  </si>
+  <si>
+    <t>define("FILE_HEADER", ROOT."header.php"); // 헤더 패스</t>
+  </si>
+  <si>
+    <t>require_once(ROOT."lib/lib_db.php"); // DB관련 라이브러리</t>
+  </si>
+  <si>
+    <t>3. Method 체크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-1. GET 일 경우 (상세 페이지의 삭제 버튼 클릭)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-2. POST일 경우 (삭제 페이지의 동의 버튼 클릭)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. DB Connect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my_db_conn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-1. connection 함수 호출</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-2. 예외 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"DB Error : PDO Instance"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-1-2. 게시글 정보 획득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>** 함수의 상세는 lib_db(DB 관련 공통)시트의 [■ DB Connect (PDO Class Instance)] 참조 **</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>db_select_boards_id</t>
+  </si>
+  <si>
+    <t>$result / false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$result = $stmt-&gt;fetchAll();</t>
+  </si>
+  <si>
+    <t>$stmt-&gt;execute($arr_ps);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예외처리 메세지 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특정 ID의 레코드 정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>■ Select rows from Boards using id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>,title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>,content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>,create_at</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FROM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>** 함수의 상세는 lib_db(DB 관련 공통)시트의 [■ Select rows from Boards using id] 참조 **</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$result = db_select_boards_id($conn, $arr_param);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-1-3. 예외 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 2-1의 처리의 리턴값이 false 일 경우, 아래 에러메세지를 출력하고 처리 종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 3-1-2의 처리 결과가 false 일 경우, 아래 메세지를 출력 후 처리 종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 3-1-2의 처리 결과의 카운트가 1건 이외 일 경우, 아래 메세지를 출력 후 처리 종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"DB Error : Select id Count"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 상기 외는 후속 처리 계속</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 상기 외는 아이템 셋팅 후, 후속 처리 계속</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$item = $result[0];</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>** 함수의 상세는 lib_db(DB 관련 공통)시트의 [■ Delete rows from Boards using id] 참조 **</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$conn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$arr_param</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PDO 객체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id =&gt; $id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-2-1. 파라미터에서 id 획득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-2-2. Transaction 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 3-2-3의 처리 결과가 false 일 경우, Rollback 후, 아래 메세지를 출력 후 처리 종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 상기 외는 Commit 후, 리스트 페이지로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>header("Location: list.php");</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exit;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-3. 공통 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>** 함수의 상세는 lib_db(DB 관련 공통)시트의 [■ DB Destroy] 참조 **</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>db_destroy_conn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>db_destroy_conn($conn);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 모든 처리 완료 후, DB 파기 처리 함수 호출</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없음 (공통 함수 파일)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동의</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>취소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Base</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. a Tag Hover</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클릭 시 삭제 처리 후, 리스트 페이지의 1페이지로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클릭 시 해당 게시글의 상세 페이지로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"id" =&gt; $id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 설정 정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my_db_conn($conn)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; id가 없을 경우, 아래 메시지를 출력 후 처리 종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Parameter Error : ID"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Array / boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"DB Error : Select id"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-1-1. 파라미터에서 id, page 획득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 파라미터가 없을 경우, 아래 메시지를 출력 후 처리 종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Parameter Error : [파라미터명]"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-2-3. 게시글 정보 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>db_delete_boards_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>특정 ID의 레코드 삭제처리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>db_delete_boards_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Array</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;$array_param</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$array_param["id"]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPDATE boards</t>
-  </si>
-  <si>
-    <t>boards</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시글 테이블</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SET</t>
-  </si>
-  <si>
-    <t>delete_at = now()</t>
-  </si>
-  <si>
-    <t>,delete_flg = 1</t>
-  </si>
-  <si>
-    <t>WHERE</t>
-  </si>
-  <si>
-    <t>id = :id</t>
-  </si>
-  <si>
-    <t>:id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. sql 작성 (UPDATE)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SQL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPDATE</t>
-  </si>
-  <si>
-    <t>2. Query 실행</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$stmt = $conn-&gt;prepare($sql);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$result = $stmt-&gt;execute($arr_ps);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prepared Statment</t>
+    <t>,delete_flg = '1'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$arr_param["id"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -304,250 +641,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3-1. Instance 생성 정상 처리 시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-2. Instance 생성 에러 발생 시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-1. [2] 까지 작업이 정상 종료 시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>retrun false;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>return $result;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-2. [2] 까지 작업에서 에러 발생 시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mini_board/src/delete.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mini_board/src/lib/lib_db.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시판 삭제 화면</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 설정 정보</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>define("ROOT", $_SERVER["DOCUMENT_ROOT"]."/mini_board/src/"); // 웹서버 root 패스 생성</t>
-  </si>
-  <si>
-    <t>define("FILE_HEADER", ROOT."header.php"); // 헤더 패스</t>
-  </si>
-  <si>
-    <t>require_once(ROOT."lib/lib_db.php"); // DB관련 라이브러리</t>
-  </si>
-  <si>
-    <t>3. Method 체크</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-1. GET 일 경우 (상세 페이지의 삭제 버튼 클릭)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-2. POST일 경우 (삭제 페이지의 동의 버튼 클릭)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. DB Connect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>my_db_conn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>my_db_conn($conn, $arr_param);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2-1. connection 함수 호출</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2-2. 예외 처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"DB Error : PDO Instance"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-1-1. 파라미터에서 id 획득</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$id = $_GET["id"];</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-1-2. 게시글 정보 획득</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>** 함수의 상세는 lib_db(DB 관련 공통)시트의 [■ DB Connect (PDO Class Instance)] 참조 **</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>db_select_boards_id</t>
-  </si>
-  <si>
-    <t>$result / false</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Array / boolen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$result = $stmt-&gt;fetchAll();</t>
-  </si>
-  <si>
-    <t>$stmt-&gt;execute($arr_ps);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예외처리 메세지 출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>특정 ID의 레코드 정보 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>■ Select rows from Boards using id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>,title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>,content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>,create_at</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FROM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>** 함수의 상세는 lib_db(DB 관련 공통)시트의 [■ Select rows from Boards using id] 참조 **</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$result = db_select_boards_id($conn, $arr_param);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-1-3. 예외 처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt; 2-1의 처리의 리턴값이 false 일 경우, 아래 에러메세지를 출력하고 처리 종료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt; 3-1-2의 처리 결과가 false 일 경우, 아래 메세지를 출력 후 처리 종료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"DB Error : Select id"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt; 3-1-2의 처리 결과의 카운트가 1건 이외 일 경우, 아래 메세지를 출력 후 처리 종료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"DB Error : Select id Count"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt; 상기 외는 후속 처리 계속</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt; 상기 외는 아이템 셋팅 후, 후속 처리 계속</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$item = $result[0];</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$id = $_POST["id"];</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>** 함수의 상세는 lib_db(DB 관련 공통)시트의 [■ Delete rows from Boards using id] 참조 **</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$result = db_delete_boards_id($conn, $arr_param);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$conn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$arr_param</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PDO 객체</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id =&gt; $id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-2-1. 파라미터에서 id 획득</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-2-2. Transaction 시작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-2-3. 게시글 정보 삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-2-3. 예외 처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt; 3-2-3의 처리 결과가 false 일 경우, Rollback 후, 아래 메세지를 출력 후 처리 종료</t>
+    <t>return false;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-2-4. 예외 처리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -555,71 +653,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&gt; 상기 외는 Commit 후, 리스트 페이지로 이동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>header("Location: list.php");</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>exit;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-3. 공통 처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>** 함수의 상세는 lib_db(DB 관련 공통)시트의 [■ DB Destroy] 참조 **</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>db_destroy_conn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>db_destroy_conn($conn);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt; 모든 처리 완료 후, DB 파기 처리 함수 호출</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>없음 (공통 함수 파일)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>취소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기능명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Base</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. a Tag Hover</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>클릭 시 삭제 처리 후, 리스트 페이지의 1페이지로 이동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>클릭 시 해당 게시글의 상세 페이지로 이동</t>
+    <t>db_delete_boards_id($conn, $arr_param)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1802,10 +1836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AM89"/>
+  <dimension ref="B1:AM91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AN31" sqref="AN31"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W77" sqref="W77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1824,7 +1858,7 @@
       <c r="D2" s="45"/>
       <c r="E2" s="44"/>
       <c r="F2" s="44" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -1862,13 +1896,13 @@
     </row>
     <row r="3" spans="2:39" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="44"/>
       <c r="D3" s="45"/>
       <c r="E3" s="44"/>
       <c r="F3" s="44" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G3" s="44"/>
       <c r="H3" s="44"/>
@@ -1912,7 +1946,7 @@
       <c r="D4" s="48"/>
       <c r="E4" s="47"/>
       <c r="F4" s="47" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G4" s="47"/>
       <c r="H4" s="47"/>
@@ -2073,7 +2107,7 @@
     <row r="8" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="42"/>
       <c r="C8" s="38" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -2094,7 +2128,7 @@
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="39" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
@@ -2836,12 +2870,12 @@
     <row r="27" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="42"/>
       <c r="C27" s="84" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D27" s="85"/>
       <c r="E27" s="86"/>
       <c r="F27" s="84" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="G27" s="85"/>
       <c r="H27" s="85"/>
@@ -2880,12 +2914,12 @@
     <row r="28" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="42"/>
       <c r="C28" s="87" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D28" s="88"/>
       <c r="E28" s="89"/>
       <c r="F28" s="78" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="G28" s="79"/>
       <c r="H28" s="79"/>
@@ -2924,12 +2958,12 @@
     <row r="29" spans="2:39" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="42"/>
       <c r="C29" s="90" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="D29" s="91"/>
       <c r="E29" s="92"/>
       <c r="F29" s="81" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="G29" s="82"/>
       <c r="H29" s="82"/>
@@ -3210,7 +3244,7 @@
     <row r="36" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="6"/>
       <c r="C36" s="38" t="s">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -3253,7 +3287,7 @@
       <c r="B37" s="6"/>
       <c r="C37" s="4"/>
       <c r="D37" s="49" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -3295,7 +3329,7 @@
       <c r="B38" s="6"/>
       <c r="C38" s="4"/>
       <c r="D38" s="49" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -3337,7 +3371,7 @@
       <c r="B39" s="6"/>
       <c r="C39" s="4"/>
       <c r="D39" s="49" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -3418,7 +3452,7 @@
     <row r="41" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="6"/>
       <c r="C41" s="39" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D41" s="37"/>
       <c r="E41" s="4"/>
@@ -3461,7 +3495,7 @@
       <c r="B42" s="6"/>
       <c r="C42" s="39"/>
       <c r="D42" s="50" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -3504,7 +3538,7 @@
       <c r="C43" s="39"/>
       <c r="D43" s="37"/>
       <c r="E43" s="4" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -3546,7 +3580,7 @@
       <c r="C44" s="4"/>
       <c r="D44" s="49"/>
       <c r="E44" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -3627,7 +3661,7 @@
       <c r="B46" s="6"/>
       <c r="C46" s="4"/>
       <c r="D46" s="50" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -3670,7 +3704,7 @@
       <c r="C47" s="4"/>
       <c r="D47" s="37"/>
       <c r="E47" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -3713,7 +3747,7 @@
       <c r="D48" s="37"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
@@ -3754,7 +3788,7 @@
       <c r="C49" s="4"/>
       <c r="D49" s="37"/>
       <c r="E49" s="4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -3834,7 +3868,7 @@
     <row r="51" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="6"/>
       <c r="C51" s="39" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D51" s="37"/>
       <c r="E51" s="4"/>
@@ -3877,7 +3911,7 @@
       <c r="B52" s="6"/>
       <c r="C52" s="4"/>
       <c r="D52" s="50" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E52" s="39"/>
       <c r="F52" s="4"/>
@@ -3920,7 +3954,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="37" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="F53" s="37"/>
       <c r="G53" s="4"/>
@@ -3963,7 +3997,7 @@
       <c r="D54" s="4"/>
       <c r="E54" s="37"/>
       <c r="F54" s="49" t="s">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
@@ -4003,11 +4037,11 @@
       <c r="B55" s="6"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
-      <c r="E55" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
@@ -4045,10 +4079,10 @@
       <c r="B56" s="6"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4" t="s">
-        <v>111</v>
-      </c>
+      <c r="E56" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="F56" s="4"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -4088,18 +4122,14 @@
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4" t="s">
-        <v>124</v>
-      </c>
+      <c r="F57" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
-      <c r="J57" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K57" s="4" t="s">
-        <v>126</v>
-      </c>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
@@ -4136,15 +4166,15 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
@@ -4180,14 +4210,18 @@
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
-      <c r="F59" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
+      <c r="J59" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
@@ -4221,10 +4255,10 @@
       <c r="B60" s="6"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
-      <c r="E60" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="F60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -4263,10 +4297,10 @@
       <c r="B61" s="6"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="E61" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="F61" s="4"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -4306,10 +4340,10 @@
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4" t="s">
-        <v>115</v>
-      </c>
+      <c r="F62" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
@@ -4348,10 +4382,10 @@
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
-      <c r="F63" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="G63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -4390,10 +4424,10 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="F64" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
@@ -4403,7 +4437,7 @@
       <c r="N64" s="4"/>
       <c r="O64" s="4"/>
       <c r="P64" s="4"/>
-      <c r="Q64" s="40"/>
+      <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
       <c r="S64" s="4"/>
       <c r="T64" s="4"/>
@@ -4432,10 +4466,10 @@
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
-      <c r="F65" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
@@ -4445,7 +4479,7 @@
       <c r="N65" s="4"/>
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
-      <c r="Q65" s="4"/>
+      <c r="Q65" s="40"/>
       <c r="R65" s="4"/>
       <c r="S65" s="4"/>
       <c r="T65" s="4"/>
@@ -4474,10 +4508,10 @@
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4" t="s">
-        <v>120</v>
-      </c>
+      <c r="F66" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
       <c r="J66" s="4"/>
@@ -4517,7 +4551,9 @@
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
+      <c r="G67" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
@@ -4554,9 +4590,7 @@
     <row r="68" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="6"/>
       <c r="C68" s="4"/>
-      <c r="D68" s="50" t="s">
-        <v>86</v>
-      </c>
+      <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
@@ -4596,11 +4630,11 @@
     <row r="69" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="6"/>
       <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="F69" s="37"/>
+      <c r="D69" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
@@ -4639,10 +4673,10 @@
       <c r="B70" s="6"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="49" t="s">
-        <v>121</v>
-      </c>
+      <c r="E70" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="F70" s="37"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
@@ -4681,10 +4715,10 @@
       <c r="B71" s="6"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
-      <c r="E71" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="F71" s="4"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="49" t="s">
+        <v>140</v>
+      </c>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
@@ -4723,11 +4757,11 @@
       <c r="B72" s="6"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
-      <c r="E72" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="49"/>
+      <c r="G72" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="J72" s="4"/>
@@ -4763,12 +4797,12 @@
     </row>
     <row r="73" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="6"/>
-      <c r="C73" s="38"/>
+      <c r="C73" s="4"/>
       <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4" t="s">
-        <v>123</v>
-      </c>
+      <c r="E73" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="F73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
@@ -4805,21 +4839,17 @@
     </row>
     <row r="74" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="6"/>
-      <c r="C74" s="38"/>
+      <c r="C74" s="4"/>
       <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
+      <c r="E74" s="37" t="s">
+        <v>147</v>
+      </c>
       <c r="F74" s="4"/>
-      <c r="G74" s="4" t="s">
-        <v>124</v>
-      </c>
+      <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
-      <c r="J74" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K74" s="4" t="s">
-        <v>126</v>
-      </c>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
       <c r="N74" s="4"/>
@@ -4854,18 +4884,14 @@
       <c r="C75" s="38"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="4" t="s">
-        <v>125</v>
-      </c>
+      <c r="F75" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
-      <c r="J75" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K75" s="4" t="s">
-        <v>127</v>
-      </c>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4"/>
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
       <c r="N75" s="4"/>
@@ -4897,17 +4923,21 @@
     </row>
     <row r="76" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="6"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="37"/>
+      <c r="C76" s="38"/>
+      <c r="D76" s="4"/>
       <c r="E76" s="4"/>
-      <c r="F76" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
-      <c r="J76" s="4"/>
-      <c r="K76" s="4"/>
+      <c r="J76" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K76" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
       <c r="N76" s="4"/>
@@ -4939,17 +4969,21 @@
     </row>
     <row r="77" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="6"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="37"/>
-      <c r="E77" s="37" t="s">
-        <v>131</v>
-      </c>
+      <c r="C77" s="38"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
       <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
+      <c r="G77" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
-      <c r="J77" s="4"/>
-      <c r="K77" s="4"/>
+      <c r="J77" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
       <c r="N77" s="4"/>
@@ -4985,7 +5019,7 @@
       <c r="D78" s="37"/>
       <c r="E78" s="4"/>
       <c r="F78" s="4" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
@@ -5025,11 +5059,11 @@
       <c r="B79" s="6"/>
       <c r="C79" s="4"/>
       <c r="D79" s="37"/>
-      <c r="E79" s="4"/>
+      <c r="E79" s="37" t="s">
+        <v>156</v>
+      </c>
       <c r="F79" s="4"/>
-      <c r="G79" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="G79" s="4"/>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
@@ -5066,10 +5100,10 @@
     <row r="80" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="6"/>
       <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
+      <c r="D80" s="37"/>
       <c r="E80" s="4"/>
       <c r="F80" s="4" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
@@ -5108,11 +5142,11 @@
     <row r="81" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="6"/>
       <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
+      <c r="D81" s="37"/>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
       <c r="G81" s="4" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
@@ -5152,10 +5186,10 @@
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4" t="s">
-        <v>136</v>
-      </c>
+      <c r="F82" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
@@ -5191,11 +5225,13 @@
     </row>
     <row r="83" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="6"/>
-      <c r="C83" s="38"/>
+      <c r="C83" s="4"/>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
+      <c r="G83" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>
@@ -5232,12 +5268,12 @@
     <row r="84" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="6"/>
       <c r="C84" s="4"/>
-      <c r="D84" s="37" t="s">
-        <v>137</v>
-      </c>
+      <c r="D84" s="4"/>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
+      <c r="G84" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
       <c r="J84" s="4"/>
@@ -5273,11 +5309,9 @@
     </row>
     <row r="85" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="6"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="4" t="s">
-        <v>141</v>
-      </c>
+      <c r="C85" s="38"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
@@ -5316,11 +5350,11 @@
     <row r="86" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" s="6"/>
       <c r="C86" s="4"/>
-      <c r="D86" s="37"/>
+      <c r="D86" s="37" t="s">
+        <v>123</v>
+      </c>
       <c r="E86" s="4"/>
-      <c r="F86" s="4" t="s">
-        <v>140</v>
-      </c>
+      <c r="F86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
@@ -5359,10 +5393,10 @@
       <c r="B87" s="6"/>
       <c r="C87" s="4"/>
       <c r="D87" s="37"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="E87" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
@@ -5402,7 +5436,9 @@
       <c r="C88" s="4"/>
       <c r="D88" s="37"/>
       <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
+      <c r="F88" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
@@ -5437,45 +5473,127 @@
       <c r="AL88" s="4"/>
       <c r="AM88" s="5"/>
     </row>
-    <row r="89" spans="2:39" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="7"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8"/>
-      <c r="I89" s="8"/>
-      <c r="J89" s="8"/>
-      <c r="K89" s="8"/>
-      <c r="L89" s="8"/>
-      <c r="M89" s="8"/>
-      <c r="N89" s="8"/>
-      <c r="O89" s="8"/>
-      <c r="P89" s="8"/>
-      <c r="Q89" s="8"/>
-      <c r="R89" s="8"/>
-      <c r="S89" s="8"/>
-      <c r="T89" s="8"/>
-      <c r="U89" s="8"/>
-      <c r="V89" s="8"/>
-      <c r="W89" s="8"/>
-      <c r="X89" s="8"/>
-      <c r="Y89" s="8"/>
-      <c r="Z89" s="8"/>
-      <c r="AA89" s="8"/>
-      <c r="AB89" s="8"/>
-      <c r="AC89" s="8"/>
-      <c r="AD89" s="8"/>
-      <c r="AE89" s="8"/>
-      <c r="AF89" s="8"/>
-      <c r="AG89" s="8"/>
-      <c r="AH89" s="8"/>
-      <c r="AI89" s="8"/>
-      <c r="AJ89" s="8"/>
-      <c r="AK89" s="8"/>
-      <c r="AL89" s="8"/>
-      <c r="AM89" s="9"/>
+    <row r="89" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="6"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="37"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="4"/>
+      <c r="O89" s="4"/>
+      <c r="P89" s="4"/>
+      <c r="Q89" s="4"/>
+      <c r="R89" s="4"/>
+      <c r="S89" s="4"/>
+      <c r="T89" s="4"/>
+      <c r="U89" s="4"/>
+      <c r="V89" s="4"/>
+      <c r="W89" s="4"/>
+      <c r="X89" s="4"/>
+      <c r="Y89" s="4"/>
+      <c r="Z89" s="4"/>
+      <c r="AA89" s="4"/>
+      <c r="AB89" s="4"/>
+      <c r="AC89" s="4"/>
+      <c r="AD89" s="4"/>
+      <c r="AE89" s="4"/>
+      <c r="AF89" s="4"/>
+      <c r="AG89" s="4"/>
+      <c r="AH89" s="4"/>
+      <c r="AI89" s="4"/>
+      <c r="AJ89" s="4"/>
+      <c r="AK89" s="4"/>
+      <c r="AL89" s="4"/>
+      <c r="AM89" s="5"/>
+    </row>
+    <row r="90" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="6"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="37"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+      <c r="M90" s="4"/>
+      <c r="N90" s="4"/>
+      <c r="O90" s="4"/>
+      <c r="P90" s="4"/>
+      <c r="Q90" s="4"/>
+      <c r="R90" s="4"/>
+      <c r="S90" s="4"/>
+      <c r="T90" s="4"/>
+      <c r="U90" s="4"/>
+      <c r="V90" s="4"/>
+      <c r="W90" s="4"/>
+      <c r="X90" s="4"/>
+      <c r="Y90" s="4"/>
+      <c r="Z90" s="4"/>
+      <c r="AA90" s="4"/>
+      <c r="AB90" s="4"/>
+      <c r="AC90" s="4"/>
+      <c r="AD90" s="4"/>
+      <c r="AE90" s="4"/>
+      <c r="AF90" s="4"/>
+      <c r="AG90" s="4"/>
+      <c r="AH90" s="4"/>
+      <c r="AI90" s="4"/>
+      <c r="AJ90" s="4"/>
+      <c r="AK90" s="4"/>
+      <c r="AL90" s="4"/>
+      <c r="AM90" s="5"/>
+    </row>
+    <row r="91" spans="2:39" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="7"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="8"/>
+      <c r="I91" s="8"/>
+      <c r="J91" s="8"/>
+      <c r="K91" s="8"/>
+      <c r="L91" s="8"/>
+      <c r="M91" s="8"/>
+      <c r="N91" s="8"/>
+      <c r="O91" s="8"/>
+      <c r="P91" s="8"/>
+      <c r="Q91" s="8"/>
+      <c r="R91" s="8"/>
+      <c r="S91" s="8"/>
+      <c r="T91" s="8"/>
+      <c r="U91" s="8"/>
+      <c r="V91" s="8"/>
+      <c r="W91" s="8"/>
+      <c r="X91" s="8"/>
+      <c r="Y91" s="8"/>
+      <c r="Z91" s="8"/>
+      <c r="AA91" s="8"/>
+      <c r="AB91" s="8"/>
+      <c r="AC91" s="8"/>
+      <c r="AD91" s="8"/>
+      <c r="AE91" s="8"/>
+      <c r="AF91" s="8"/>
+      <c r="AG91" s="8"/>
+      <c r="AH91" s="8"/>
+      <c r="AI91" s="8"/>
+      <c r="AJ91" s="8"/>
+      <c r="AK91" s="8"/>
+      <c r="AL91" s="8"/>
+      <c r="AM91" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -5489,8 +5607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AM119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD9" sqref="AD9"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="AA115" sqref="AA115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5547,7 +5665,7 @@
     </row>
     <row r="3" spans="2:39" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="44"/>
       <c r="D3" s="45"/>
@@ -5597,7 +5715,7 @@
       <c r="D4" s="48"/>
       <c r="E4" s="47"/>
       <c r="F4" s="47" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G4" s="47"/>
       <c r="H4" s="47"/>
@@ -5758,7 +5876,7 @@
     <row r="8" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="42"/>
       <c r="C8" s="4" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -6005,15 +6123,15 @@
       <c r="B14" s="6"/>
       <c r="C14" s="4"/>
       <c r="D14" s="37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -6051,15 +6169,15 @@
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
       <c r="D15" s="37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -6097,20 +6215,20 @@
       <c r="B16" s="6"/>
       <c r="C16" s="4"/>
       <c r="D16" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -6150,15 +6268,15 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
@@ -6193,12 +6311,12 @@
       <c r="B18" s="6"/>
       <c r="C18" s="4"/>
       <c r="D18" s="37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -6238,7 +6356,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="39" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -6281,7 +6399,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -6324,16 +6442,16 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -6370,16 +6488,16 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
@@ -6416,16 +6534,16 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -6462,16 +6580,16 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
@@ -6508,16 +6626,16 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -6593,7 +6711,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -6636,7 +6754,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
@@ -6647,10 +6765,10 @@
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q28" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
@@ -6682,7 +6800,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
@@ -6693,10 +6811,10 @@
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q29" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
@@ -6728,7 +6846,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
@@ -6739,10 +6857,10 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
@@ -6812,7 +6930,7 @@
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -6894,7 +7012,7 @@
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="39" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -6937,7 +7055,7 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="37" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -6980,7 +7098,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -7022,7 +7140,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -7063,7 +7181,7 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="37" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -7106,7 +7224,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
@@ -7148,7 +7266,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
@@ -7266,7 +7384,7 @@
     <row r="43" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="6"/>
       <c r="C43" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -7309,15 +7427,15 @@
       <c r="B44" s="6"/>
       <c r="C44" s="4"/>
       <c r="D44" s="37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -7355,15 +7473,15 @@
       <c r="B45" s="6"/>
       <c r="C45" s="4"/>
       <c r="D45" s="37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -7401,20 +7519,20 @@
       <c r="B46" s="6"/>
       <c r="C46" s="4"/>
       <c r="D46" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
@@ -7454,10 +7572,10 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -7495,12 +7613,12 @@
       <c r="B48" s="6"/>
       <c r="C48" s="4"/>
       <c r="D48" s="37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
@@ -7540,7 +7658,7 @@
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -7583,7 +7701,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
@@ -7702,7 +7820,7 @@
     <row r="53" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="6"/>
       <c r="C53" s="38" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -7745,15 +7863,15 @@
       <c r="B54" s="6"/>
       <c r="C54" s="4"/>
       <c r="D54" s="37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
@@ -7791,15 +7909,15 @@
       <c r="B55" s="6"/>
       <c r="C55" s="4"/>
       <c r="D55" s="37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
@@ -7837,20 +7955,20 @@
       <c r="B56" s="6"/>
       <c r="C56" s="4"/>
       <c r="D56" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="L56" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
@@ -7888,12 +8006,12 @@
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="L57" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
@@ -7932,15 +8050,15 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="L58" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
@@ -7974,12 +8092,12 @@
       <c r="B59" s="6"/>
       <c r="C59" s="4"/>
       <c r="D59" s="37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -8019,7 +8137,7 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="39" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -8062,7 +8180,7 @@
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="51" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G61" s="52"/>
       <c r="H61" s="52"/>
@@ -8071,7 +8189,7 @@
       <c r="K61" s="53"/>
       <c r="L61" s="54"/>
       <c r="M61" s="52" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="N61" s="52"/>
       <c r="O61" s="52"/>
@@ -8106,7 +8224,7 @@
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="56" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G62" s="57"/>
       <c r="H62" s="57"/>
@@ -8115,12 +8233,12 @@
       <c r="K62" s="58"/>
       <c r="L62" s="59"/>
       <c r="M62" s="57" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N62" s="57"/>
       <c r="O62" s="57"/>
       <c r="P62" s="52" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q62" s="57"/>
       <c r="R62" s="57"/>
@@ -8152,7 +8270,7 @@
       <c r="D63" s="4"/>
       <c r="E63" s="39"/>
       <c r="F63" s="61" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G63" s="62"/>
       <c r="H63" s="62"/>
@@ -8161,13 +8279,13 @@
       <c r="K63" s="63"/>
       <c r="L63" s="64"/>
       <c r="M63" s="62" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N63" s="62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O63" s="62" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="P63" s="62"/>
       <c r="Q63" s="62"/>
@@ -8200,7 +8318,7 @@
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
       <c r="F64" s="66" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G64" s="67"/>
       <c r="H64" s="67"/>
@@ -8249,7 +8367,7 @@
       <c r="K65" s="72"/>
       <c r="L65" s="69"/>
       <c r="M65" s="69" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="N65" s="69"/>
       <c r="O65" s="69"/>
@@ -8292,7 +8410,7 @@
       <c r="L66" s="69"/>
       <c r="M66" s="69"/>
       <c r="N66" s="69" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="O66" s="69"/>
       <c r="P66" s="69"/>
@@ -8334,7 +8452,7 @@
       <c r="L67" s="69"/>
       <c r="M67" s="69"/>
       <c r="N67" s="69" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="O67" s="69"/>
       <c r="P67" s="69"/>
@@ -8376,7 +8494,7 @@
       <c r="L68" s="69"/>
       <c r="M68" s="69"/>
       <c r="N68" s="69" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="O68" s="69"/>
       <c r="P68" s="69"/>
@@ -8418,7 +8536,7 @@
       <c r="L69" s="69"/>
       <c r="M69" s="69"/>
       <c r="N69" s="69" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="O69" s="69"/>
       <c r="P69" s="69"/>
@@ -8459,7 +8577,7 @@
       <c r="K70" s="72"/>
       <c r="L70" s="69"/>
       <c r="M70" s="69" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="N70" s="69"/>
       <c r="O70" s="69"/>
@@ -8502,7 +8620,7 @@
       <c r="L71" s="69"/>
       <c r="M71" s="69"/>
       <c r="N71" s="69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="O71" s="69"/>
       <c r="P71" s="69"/>
@@ -8543,7 +8661,7 @@
       <c r="K72" s="72"/>
       <c r="L72" s="69"/>
       <c r="M72" s="69" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N72" s="69"/>
       <c r="O72" s="69"/>
@@ -8586,7 +8704,7 @@
       <c r="L73" s="69"/>
       <c r="M73" s="69"/>
       <c r="N73" s="69" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="O73" s="69"/>
       <c r="P73" s="69"/>
@@ -8699,7 +8817,7 @@
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="39" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
@@ -8742,7 +8860,7 @@
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
       <c r="F77" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
@@ -8784,7 +8902,7 @@
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
       <c r="F78" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
@@ -8826,7 +8944,7 @@
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
       <c r="F79" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
@@ -8907,7 +9025,7 @@
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="39" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
@@ -8950,7 +9068,7 @@
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
       <c r="F82" s="37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
@@ -8993,7 +9111,7 @@
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
@@ -9034,7 +9152,7 @@
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
       <c r="F84" s="37" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
@@ -9077,7 +9195,7 @@
       <c r="E85" s="4"/>
       <c r="F85" s="37"/>
       <c r="G85" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
@@ -9119,7 +9237,7 @@
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
@@ -9237,7 +9355,7 @@
     <row r="89" spans="2:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="6"/>
       <c r="C89" s="38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -9280,15 +9398,15 @@
       <c r="B90" s="6"/>
       <c r="C90" s="4"/>
       <c r="D90" s="37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
       <c r="G90" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="I90" s="4"/>
       <c r="J90" s="4"/>
@@ -9326,15 +9444,15 @@
       <c r="B91" s="6"/>
       <c r="C91" s="4"/>
       <c r="D91" s="37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
       <c r="G91" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>46</v>
+        <v>148</v>
       </c>
       <c r="I91" s="4"/>
       <c r="J91" s="4"/>
@@ -9372,20 +9490,20 @@
       <c r="B92" s="6"/>
       <c r="C92" s="4"/>
       <c r="D92" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
       <c r="G92" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I92" s="4"/>
       <c r="J92" s="4"/>
       <c r="K92" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
@@ -9424,12 +9542,12 @@
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I93" s="4"/>
       <c r="J93" s="4"/>
       <c r="K93" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
@@ -9469,15 +9587,15 @@
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
       <c r="G94" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H94" s="4" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
       <c r="I94" s="4"/>
       <c r="J94" s="4"/>
       <c r="K94" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L94" s="4"/>
       <c r="M94" s="4"/>
@@ -9512,12 +9630,12 @@
       <c r="B95" s="6"/>
       <c r="C95" s="4"/>
       <c r="D95" s="37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
       <c r="G95" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
@@ -9557,7 +9675,7 @@
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
       <c r="E96" s="39" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
@@ -9600,7 +9718,7 @@
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
       <c r="F97" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
@@ -9609,7 +9727,7 @@
       <c r="K97" s="12"/>
       <c r="L97" s="26"/>
       <c r="M97" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="N97" s="11"/>
       <c r="O97" s="11"/>
@@ -9644,7 +9762,7 @@
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
       <c r="F98" s="32" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G98" s="33"/>
       <c r="H98" s="33"/>
@@ -9653,12 +9771,12 @@
       <c r="K98" s="34"/>
       <c r="L98" s="35"/>
       <c r="M98" s="33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N98" s="33"/>
       <c r="O98" s="33"/>
       <c r="P98" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q98" s="33"/>
       <c r="R98" s="33"/>
@@ -9690,7 +9808,7 @@
       <c r="D99" s="4"/>
       <c r="E99" s="39"/>
       <c r="F99" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G99" s="14"/>
       <c r="H99" s="14"/>
@@ -9699,13 +9817,13 @@
       <c r="K99" s="15"/>
       <c r="L99" s="28"/>
       <c r="M99" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N99" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O99" s="14" t="s">
-        <v>52</v>
+        <v>151</v>
       </c>
       <c r="P99" s="14"/>
       <c r="Q99" s="14"/>
@@ -9738,7 +9856,7 @@
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
       <c r="F100" s="16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G100" s="17"/>
       <c r="H100" s="17"/>
@@ -9787,7 +9905,7 @@
       <c r="K101" s="21"/>
       <c r="L101" s="20"/>
       <c r="M101" s="20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N101" s="20"/>
       <c r="O101" s="20"/>
@@ -9829,7 +9947,7 @@
       <c r="K102" s="21"/>
       <c r="L102" s="20"/>
       <c r="M102" s="20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N102" s="20"/>
       <c r="O102" s="20"/>
@@ -9872,7 +9990,7 @@
       <c r="L103" s="20"/>
       <c r="M103" s="20"/>
       <c r="N103" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="O103" s="20"/>
       <c r="P103" s="20"/>
@@ -9914,7 +10032,7 @@
       <c r="L104" s="20"/>
       <c r="M104" s="20"/>
       <c r="N104" s="20" t="s">
-        <v>58</v>
+        <v>150</v>
       </c>
       <c r="O104" s="20"/>
       <c r="P104" s="20"/>
@@ -9955,7 +10073,7 @@
       <c r="K105" s="21"/>
       <c r="L105" s="20"/>
       <c r="M105" s="20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N105" s="20"/>
       <c r="O105" s="20"/>
@@ -9998,7 +10116,7 @@
       <c r="L106" s="20"/>
       <c r="M106" s="20"/>
       <c r="N106" s="20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="O106" s="20"/>
       <c r="P106" s="20"/>
@@ -10111,7 +10229,7 @@
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="39" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
@@ -10154,7 +10272,7 @@
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
       <c r="F110" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
@@ -10196,7 +10314,7 @@
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
       <c r="F111" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
@@ -10277,7 +10395,7 @@
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="39" t="s">
-        <v>69</v>
+        <v>154</v>
       </c>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
@@ -10320,7 +10438,7 @@
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
       <c r="F114" s="37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
@@ -10363,7 +10481,7 @@
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
       <c r="G115" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
@@ -10404,7 +10522,7 @@
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
       <c r="F116" s="37" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
@@ -10447,7 +10565,7 @@
       <c r="E117" s="4"/>
       <c r="F117" s="37"/>
       <c r="G117" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
@@ -10489,7 +10607,7 @@
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
       <c r="G118" s="4" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
@@ -10567,5 +10685,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>